<commit_message>
Finished reading chapter 1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26040" yWindow="1180" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -549,7 +549,9 @@
       <c r="B3" s="1">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41775</v>
       </c>
@@ -734,7 +736,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished skeleton of week 1 DQ1
Still need to elaborate more and reword.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-27340" yWindow="540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -106,6 +106,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -502,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -563,7 +564,9 @@
       <c r="B4" s="1">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D4" s="2">
         <v>41776</v>
       </c>
@@ -575,7 +578,9 @@
       <c r="B5" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
       <c r="D5" s="2">
         <v>41776</v>
       </c>
@@ -736,7 +741,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>2.8472222222222218E-2</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished skeleton of week 1 DQ2
Still need to elaborate, add examples, and re-word.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -592,7 +592,9 @@
       <c r="B6" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>4.7222222222222221E-2</v>
+      </c>
       <c r="D6" s="2">
         <v>41777</v>
       </c>
@@ -654,7 +656,9 @@
       <c r="B12" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>3.125E-2</v>
+      </c>
       <c r="D12" s="2">
         <v>41777</v>
       </c>
@@ -741,7 +745,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>2.8472222222222218E-2</v>
+        <v>0.10694444444444444</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 1 DQ1
Still need to proofread
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27340" yWindow="540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="19080" yWindow="3400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,7 +593,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C6" s="1">
-        <v>4.7222222222222221E-2</v>
+        <v>8.0555555555555561E-2</v>
       </c>
       <c r="D6" s="2">
         <v>41777</v>
@@ -745,7 +745,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.10694444444444444</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 1 DQ2
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="3400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8280" yWindow="5600" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,7 +657,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C12" s="1">
-        <v>3.125E-2</v>
+        <v>9.3055555555555558E-2</v>
       </c>
       <c r="D12" s="2">
         <v>41777</v>
@@ -745,7 +745,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.14027777777777778</v>
+        <v>0.20208333333333334</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to the first post.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="5600" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-27820" yWindow="760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,7 +606,9 @@
       <c r="B7" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5">
@@ -745,7 +747,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.20208333333333334</v>
+        <v>0.20902777777777778</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to first post while at work on 5/19/2014
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27820" yWindow="760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="38220" windowHeight="15375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,11 +96,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,17 +499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -672,7 +672,9 @@
       <c r="B13" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5">
@@ -747,7 +749,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.20902777777777778</v>
+        <v>0.21597222222222223</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
More than halfway through assignment 1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="38220" windowHeight="15375" tabRatio="500"/>
+    <workbookView xWindow="-24300" yWindow="1140" windowWidth="23120" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,11 +96,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,17 +499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Responded to first post of May 20
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -618,7 +618,9 @@
       <c r="B8" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5">
@@ -749,7 +751,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.21597222222222223</v>
+        <v>0.22291666666666668</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to more posts.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24300" yWindow="1140" windowWidth="23120" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="18315" windowHeight="10695" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,11 +96,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,17 +499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -630,7 +630,9 @@
       <c r="B9" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5">
@@ -640,7 +642,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5">
@@ -751,7 +755,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.22291666666666668</v>
+        <v>0.24027777777777778</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
assigment 1 mostly done.
Just need to add comments.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="18315" windowHeight="10695" tabRatio="500"/>
+    <workbookView xWindow="10540" yWindow="3660" windowWidth="18320" windowHeight="10700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,11 +96,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,17 +499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -690,7 +690,9 @@
       <c r="B14" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:5">
@@ -700,7 +702,9 @@
       <c r="B15" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5">
@@ -755,7 +759,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.24027777777777778</v>
+        <v>0.27152777777777781</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Completed 5 replies for both DQs of week 1.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="3660" windowWidth="18320" windowHeight="10700" tabRatio="500"/>
+    <workbookView xWindow="210" yWindow="495" windowWidth="18315" windowHeight="10695" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>DQ2 response 5</t>
-  </si>
-  <si>
-    <t>DQ2 response 6</t>
   </si>
   <si>
     <t>Hand-in assignment</t>
@@ -96,11 +93,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,17 +496,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -545,7 +542,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>5.5555555555555552E-2</v>
@@ -559,7 +556,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>5.2083333333333336E-2</v>
@@ -573,7 +570,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>3.125E-2</v>
@@ -654,7 +651,9 @@
       <c r="B11" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5">
@@ -714,7 +713,9 @@
       <c r="B16" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
@@ -724,7 +725,9 @@
       <c r="B17" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
@@ -732,36 +735,26 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="4">
+        <v>41780</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4">
-        <v>41780</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUM(B2:B19)</f>
+        <f>SUM(B2:B18)</f>
         <v>0.71527777777777768</v>
       </c>
-      <c r="C20" s="1">
-        <f>SUM(C2:C19)</f>
-        <v>0.27152777777777781</v>
-      </c>
-      <c r="D20" s="2"/>
+      <c r="C19" s="1">
+        <f>SUM(C2:C18)</f>
+        <v>0.2993055555555556</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Almost done with assignment 1
Need to rename files, zip, and submit.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -737,7 +737,9 @@
       <c r="B18" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>0.25</v>
+      </c>
       <c r="D18" s="4">
         <v>41780</v>
       </c>
@@ -752,7 +754,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.2993055555555556</v>
+        <v>0.5493055555555556</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created week 2 schedule
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="495" windowWidth="18315" windowHeight="10695" tabRatio="500"/>
+    <workbookView xWindow="13820" yWindow="580" windowWidth="32000" windowHeight="22640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
+    <sheet name="week2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -88,22 +89,31 @@
   </si>
   <si>
     <t>Read Sections 4.1-4.5</t>
+  </si>
+  <si>
+    <t>Read Sections 2.10-2.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Sections 4.8-4.12 </t>
+  </si>
+  <si>
+    <t>Read Sections Sections 5.1-5.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -147,8 +157,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,11 +197,35 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,17 +554,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -755,6 +813,268 @@
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
         <v>0.5493055555555556</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41784</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2">
+        <v>41784</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2">
+        <v>41785</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>41786</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <f>SUM(B2:B18)</f>
+        <v>0.63888888888888906</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(C4:C18)</f>
+        <v>0</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created skeleton of week 2 DQ1
Still need to reword.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -867,7 +867,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>6.25E-2</v>
+      </c>
       <c r="D2" s="2">
         <v>41783</v>
       </c>

</xml_diff>

<commit_message>
Finished draft of week 2 DQ1
Still need to proof-read.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13820" yWindow="580" windowWidth="32000" windowHeight="22640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9020" yWindow="2560" windowWidth="32000" windowHeight="22640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>6.25E-2</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="D2" s="2">
         <v>41783</v>
@@ -881,7 +881,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>5.2083333333333336E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41784</v>
       </c>
@@ -1075,8 +1077,8 @@
         <v>0.63888888888888906</v>
       </c>
       <c r="C19" s="1">
-        <f>SUM(C4:C18)</f>
-        <v>0</v>
+        <f>SUM(C2:C18)</f>
+        <v>0.1701388888888889</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Started rewording week 2 DQ2 notes
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -882,7 +882,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>5.2083333333333336E-2</v>
+        <v>5.6944444444444443E-2</v>
       </c>
       <c r="D3" s="2">
         <v>41784</v>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.1701388888888889</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Week 2 DQs submitted.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -882,7 +882,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>5.6944444444444443E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D3" s="2">
         <v>41784</v>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.17500000000000002</v>
+        <v>0.2638888888888889</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made 2 first replies for week 2
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -943,7 +943,9 @@
       <c r="B8" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D8" s="2">
         <v>41784</v>
       </c>
@@ -1003,7 +1005,9 @@
       <c r="B13" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D13" s="2">
         <v>41784</v>
       </c>
@@ -1078,7 +1082,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.2638888888888889</v>
+        <v>0.28472222222222227</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished week 2 reading
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9020" yWindow="2560" windowWidth="32000" windowHeight="22640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -832,7 +832,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -895,7 +895,9 @@
       <c r="B4" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D4" s="2">
         <v>41785</v>
       </c>
@@ -907,7 +909,9 @@
       <c r="B5" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D5" s="2">
         <v>41785</v>
       </c>
@@ -919,7 +923,9 @@
       <c r="B6" s="1">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="D6" s="2">
         <v>41785</v>
       </c>
@@ -931,7 +937,9 @@
       <c r="B7" s="1">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
       <c r="D7" s="2">
         <v>41785</v>
       </c>
@@ -1082,7 +1090,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.28472222222222227</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created 2 sections separate for assignment 2
Need to fix section 1 and create new html doc with 2 divs
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -832,7 +832,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1075,7 +1075,9 @@
       <c r="B18" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="D18" s="4">
         <v>41787</v>
       </c>
@@ -1090,7 +1092,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.33750000000000002</v>
+        <v>0.54583333333333339</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Replied to more posts.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -103,11 +103,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,17 +554,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -828,17 +828,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -979,7 +979,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41785</v>
       </c>
@@ -991,7 +993,9 @@
       <c r="B11" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D11" s="2">
         <v>41786</v>
       </c>
@@ -1043,7 +1047,9 @@
       <c r="B15" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D15" s="2">
         <v>41785</v>
       </c>
@@ -1096,7 +1102,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.6118055555555556</v>
+        <v>0.65000000000000013</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
week 2 assignment submitted
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-28320" yWindow="600" windowWidth="27240" windowHeight="15860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -103,11 +103,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,17 +554,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -828,17 +828,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1061,7 +1061,9 @@
       <c r="B16" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D16" s="2">
         <v>41786</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="C18" s="1">
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D18" s="4">
         <v>41787</v>
@@ -1102,7 +1104,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.65000000000000013</v>
+        <v>0.74375000000000013</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Week 3 schedule completed
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="600" windowWidth="27240" windowHeight="15860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="24750" windowHeight="11730" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
+    <sheet name="week3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -98,16 +99,28 @@
   </si>
   <si>
     <t>Read Sections Sections 5.1-5.5</t>
+  </si>
+  <si>
+    <t>Read Sections 7.1-7.6</t>
+  </si>
+  <si>
+    <t>Read Sections 12.1-12.2</t>
+  </si>
+  <si>
+    <t>Read Sections Sections 13.1-13.9</t>
+  </si>
+  <si>
+    <t>Group assignment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,17 +567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -828,17 +841,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1117,4 +1130,260 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <f>SUM(B2:B18)</f>
+        <v>0.74652777777777757</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(C2:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished skeleton of week 3 DQ1
Still need to reword.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24750" windowHeight="11730" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-26060" yWindow="1200" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -116,11 +116,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -567,17 +567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -841,17 +841,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1133,19 +1133,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1172,7 +1172,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>3.6805555555555557E-2</v>
+      </c>
       <c r="D2" s="2">
         <v>41791</v>
       </c>
@@ -1379,11 +1381,16 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0</v>
+        <v>3.6805555555555557E-2</v>
       </c>
       <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished skeleton of week 3 DQ2
Still need to reword and organize.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1186,7 +1186,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>5.347222222222222E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41791</v>
       </c>
@@ -1381,7 +1383,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>3.6805555555555557E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 3 DQ1
Still need to proof read.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1173,7 +1173,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>3.6805555555555557E-2</v>
+        <v>7.013888888888889E-2</v>
       </c>
       <c r="D2" s="2">
         <v>41791</v>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>9.0277777777777776E-2</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 3 DQ2
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26060" yWindow="1200" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="15280" yWindow="600" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1187,7 +1187,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>5.347222222222222E-2</v>
+        <v>0.1013888888888889</v>
       </c>
       <c r="D3" s="2">
         <v>41791</v>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.12361111111111112</v>
+        <v>0.17152777777777778</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
First version of assignment 3 done.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15280" yWindow="600" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-27000" yWindow="1800" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -170,8 +170,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -210,7 +212,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -225,6 +227,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +242,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1137,7 +1141,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1200,7 +1204,6 @@
       <c r="B4" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="2">
         <v>41792</v>
       </c>
@@ -1248,7 +1251,9 @@
       <c r="B8" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D8" s="2">
         <v>41792</v>
       </c>
@@ -1308,7 +1313,9 @@
       <c r="B13" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D13" s="2">
         <v>41792</v>
       </c>
@@ -1383,12 +1390,13 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.17152777777777778</v>
+        <v>0.19583333333333333</v>
       </c>
       <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Completed version 0.1 of about us page for week 3
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27000" yWindow="1800" windowWidth="23380" windowHeight="13960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Group assignment</t>
+  </si>
+  <si>
+    <t>Left of at page 4</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1144,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1207,6 +1210,9 @@
       <c r="D4" s="2">
         <v>41792</v>
       </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1215,7 +1221,9 @@
       <c r="B5" s="1">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="D5" s="2">
         <v>41792</v>
       </c>
@@ -1227,7 +1235,9 @@
       <c r="B6" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="D6" s="2">
         <v>41792</v>
       </c>
@@ -1390,7 +1400,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.19583333333333333</v>
+        <v>0.20277777777777775</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to another post.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="17280" yWindow="3760" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -119,11 +119,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -574,17 +574,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -848,17 +848,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1140,19 +1140,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1289,7 +1289,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41793</v>
       </c>
@@ -1404,7 +1406,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.23749999999999999</v>
+        <v>0.25138888888888888</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
There are now 3 responses for each DQ
Still need to do 2 more for each.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="3760" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1785" yWindow="285" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -119,11 +119,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -574,17 +574,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -848,17 +848,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1140,19 +1140,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1355,7 +1355,9 @@
       <c r="B15" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D15" s="2">
         <v>41793</v>
       </c>
@@ -1406,7 +1408,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.25138888888888888</v>
+        <v>0.26180555555555557</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of statement
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1393,7 +1393,9 @@
       <c r="B18" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>0.25</v>
+      </c>
       <c r="D18" s="4">
         <v>41794</v>
       </c>
@@ -1408,7 +1410,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.26180555555555557</v>
+        <v>0.51180555555555562</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Week 3 assignment submitted.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1303,7 +1303,9 @@
       <c r="B11" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D11" s="2">
         <v>41794</v>
       </c>
@@ -1315,7 +1317,9 @@
       <c r="B12" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D12" s="2">
         <v>41794</v>
       </c>
@@ -1369,7 +1373,9 @@
       <c r="B16" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D16" s="2">
         <v>41794</v>
       </c>
@@ -1381,7 +1387,9 @@
       <c r="B17" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D17" s="2">
         <v>41794</v>
       </c>
@@ -1410,7 +1418,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.51180555555555562</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
First try at fixing
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="285" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1780" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -111,19 +111,16 @@
   </si>
   <si>
     <t>Group assignment</t>
-  </si>
-  <si>
-    <t>Left of at page 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,7 +203,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -214,6 +211,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -574,17 +572,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -848,17 +846,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1140,19 +1138,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1207,11 +1205,11 @@
       <c r="B4" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
+      <c r="C4" s="5">
+        <v>3.125E-2</v>
+      </c>
       <c r="D4" s="2">
         <v>41792</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1249,7 +1247,9 @@
       <c r="B7" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D7" s="2">
         <v>41792</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.56041666666666667</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created week 4 plan
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="17720" yWindow="4580" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
+    <sheet name="week4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -111,6 +112,21 @@
   </si>
   <si>
     <t>Group assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Sections 7.7-7.13 </t>
+  </si>
+  <si>
+    <t>Read Sections 8.1-8.9</t>
+  </si>
+  <si>
+    <t>Read Sections 9.1-9.4</t>
+  </si>
+  <si>
+    <t>Read Sections 10.1-10.4</t>
+  </si>
+  <si>
+    <t>Read Section 11.1-11.3</t>
   </si>
 </sst>
 </file>
@@ -170,8 +186,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +245,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -229,6 +261,14 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -244,6 +284,14 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1141,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1431,4 +1479,290 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2">
+        <v>41799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <f>SUM(B2:B20)</f>
+        <v>0.86458333333333293</v>
+      </c>
+      <c r="C21" s="1">
+        <f>SUM(C2:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first version of skeleton for week 4 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="17720" yWindow="4580" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1521,7 +1521,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="D2" s="2">
         <v>41432</v>
       </c>
@@ -1752,7 +1754,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Started draft of week 4 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="4580" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2300" yWindow="4580" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1535,7 +1535,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41432</v>
       </c>
@@ -1754,7 +1756,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.10416666666666667</v>
+        <v>0.1875</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 4 DQ2
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="4580" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="10380" yWindow="1300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1522,7 +1522,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>0.10416666666666667</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D2" s="2">
         <v>41432</v>
@@ -1536,7 +1536,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D3" s="2">
         <v>41432</v>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.1875</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished reading week 4 lecture notes.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="1300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2200" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1549,7 +1549,9 @@
       <c r="B4" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D4" s="2">
         <v>41798</v>
       </c>
@@ -1756,7 +1758,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to 2 posts today.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2235" yWindow="3480" windowWidth="25605" windowHeight="9405" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -132,11 +132,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -620,17 +620,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -894,17 +894,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1186,19 +1186,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1482,17 +1482,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1623,7 +1623,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41799</v>
       </c>
@@ -1683,7 +1685,9 @@
       <c r="B15" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D15" s="2">
         <v>41799</v>
       </c>
@@ -1758,7 +1762,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.33333333333333337</v>
+        <v>0.35416666666666674</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to first post of the day
Still need to make at least one more today.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25540" yWindow="120" windowWidth="24340" windowHeight="18540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25710" windowHeight="10335" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -135,11 +135,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -623,17 +623,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -897,17 +897,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1189,19 +1189,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1485,17 +1485,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1644,7 +1644,9 @@
       <c r="B11" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D11" s="2">
         <v>41800</v>
       </c>
@@ -1769,7 +1771,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.36805555555555564</v>
+        <v>0.38194444444444453</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made last post for 6/10
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25710" windowHeight="10335" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22220" windowHeight="14840" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -135,11 +135,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -623,17 +623,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -897,17 +897,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1189,19 +1189,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1485,17 +1485,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1708,7 +1708,9 @@
       <c r="B16" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D16" s="2">
         <v>41800</v>
       </c>
@@ -1771,7 +1773,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.38194444444444453</v>
+        <v>0.40277777777777785</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
filled out week 4 tasks
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="1600" windowWidth="22220" windowHeight="14840" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1489,7 +1489,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1765,7 +1765,7 @@
         <v>0.25</v>
       </c>
       <c r="C20" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.625</v>
       </c>
       <c r="D20" s="4">
         <v>41801</v>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C21" s="1">
         <f>SUM(C2:C20)</f>
-        <v>0.90972222222222232</v>
+        <v>1.0763888888888888</v>
       </c>
       <c r="D21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Created week 5 plan
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="24060" yWindow="3800" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
     <sheet name="week2" sheetId="2" r:id="rId2"/>
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week4" sheetId="4" r:id="rId4"/>
+    <sheet name="week5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -130,6 +131,18 @@
   </si>
   <si>
     <t>Assignment</t>
+  </si>
+  <si>
+    <t>Read Sections 17.1-17.6</t>
+  </si>
+  <si>
+    <t>Read Sections 19.1-19.8</t>
+  </si>
+  <si>
+    <t>Read Section 19.10</t>
+  </si>
+  <si>
+    <t>Read Section 19.12</t>
   </si>
 </sst>
 </file>
@@ -189,8 +202,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,7 +275,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -272,6 +299,13 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -295,6 +329,13 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1488,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1794,4 +1835,278 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41807</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2">
+        <v>41805</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2">
+        <v>41806</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>41807</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <f>SUM(B2:B19)</f>
+        <v>0.83680555555555525</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C2:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished skeleton of week 5 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="3800" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="10000" yWindow="3880" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1842,7 +1842,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1877,7 +1877,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>6.8749999999999992E-2</v>
+      </c>
       <c r="D2" s="2">
         <v>41804</v>
       </c>
@@ -2096,7 +2098,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0</v>
+        <v>6.8749999999999992E-2</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 5 DQ1
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="3880" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="26560" yWindow="3840" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1842,7 +1842,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1891,7 +1891,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41804</v>
       </c>
@@ -2098,7 +2100,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>6.8749999999999992E-2</v>
+        <v>0.11041666666666666</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 5 DQ2
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26560" yWindow="3840" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="12460" yWindow="3900" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1878,7 +1878,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>6.8749999999999992E-2</v>
+        <v>0.11041666666666666</v>
       </c>
       <c r="D2" s="2">
         <v>41804</v>
@@ -1892,7 +1892,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>9.8611111111111108E-2</v>
       </c>
       <c r="D3" s="2">
         <v>41804</v>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.11041666666666666</v>
+        <v>0.20902777777777776</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to second post.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12460" yWindow="3900" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="315" yWindow="30" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="week4" sheetId="4" r:id="rId4"/>
     <sheet name="week5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -148,11 +148,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -664,17 +664,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -938,17 +938,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1230,19 +1230,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1526,17 +1526,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1838,17 +1838,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2027,7 +2027,9 @@
       <c r="B14" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D14" s="2">
         <v>41805</v>
       </c>
@@ -2102,7 +2104,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.22291666666666665</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
validation added to about us page.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="30" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="320" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="week4" sheetId="4" r:id="rId4"/>
     <sheet name="week5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -148,11 +148,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -664,17 +664,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -938,17 +938,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1230,19 +1230,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1526,17 +1526,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1838,17 +1838,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1979,7 +1979,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41806</v>
       </c>
@@ -2104,7 +2106,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.23333333333333331</v>
+        <v>0.24374999999999997</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added color functionality to assignment 5.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1842,7 +1842,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2059,7 +2059,9 @@
       <c r="B16" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D16" s="2">
         <v>41807</v>
       </c>
@@ -2112,7 +2114,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.35138888888888886</v>
+        <v>0.36180555555555555</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Completed week 5 individual statement
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1842,7 +1842,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2098,7 +2098,7 @@
         <v>0.25</v>
       </c>
       <c r="C19" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.25</v>
       </c>
       <c r="D19" s="4">
         <v>41808</v>
@@ -2114,7 +2114,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.36180555555555555</v>
+        <v>0.52847222222222223</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
week 5 assignment submitted
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1842,7 +1842,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2007,7 +2007,9 @@
       <c r="B12" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D12" s="2">
         <v>41808</v>
       </c>
@@ -2073,7 +2075,9 @@
       <c r="B17" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D17" s="2">
         <v>41808</v>
       </c>
@@ -2114,7 +2118,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.52847222222222223</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="D20" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made week 6 schedule
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="45" windowWidth="19140" windowHeight="10065" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="25760" yWindow="5800" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="week3" sheetId="3" r:id="rId3"/>
     <sheet name="week4" sheetId="4" r:id="rId4"/>
     <sheet name="week5" sheetId="5" r:id="rId5"/>
+    <sheet name="week6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -143,16 +144,22 @@
   </si>
   <si>
     <t>Read Section 19.12</t>
+  </si>
+  <si>
+    <t>Read Sections 18.1-18.5</t>
+  </si>
+  <si>
+    <t>Read 19.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,8 +209,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,7 +296,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -306,6 +327,13 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +364,13 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,17 +699,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -938,17 +973,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1230,19 +1265,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1526,17 +1561,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1838,17 +1873,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C18" sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2121,6 +2156,250 @@
         <v>0.55625000000000002</v>
       </c>
       <c r="D20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41811</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41811</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41814</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41815</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2">
+        <v>41812</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2">
+        <v>41812</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2">
+        <v>41813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2">
+        <v>41814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>41815</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4">
+        <v>41815</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <f>SUM(B2:B17)</f>
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUM(C2:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finished skeleton of week 6 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2173,7 +2173,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2208,7 +2208,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D2" s="2">
         <v>41811</v>
       </c>
@@ -2397,7 +2399,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 6 DQ2
Still need to proof-read.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25760" yWindow="5800" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="6960" yWindow="3660" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -2173,7 +2173,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2222,7 +2222,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41811</v>
       </c>
@@ -2399,7 +2401,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 6 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2173,7 +2173,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2209,7 +2209,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>7.5694444444444439E-2</v>
       </c>
       <c r="D2" s="2">
         <v>41811</v>
@@ -2223,7 +2223,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="D3" s="2">
         <v>41811</v>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.22777777777777775</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished up reading from week 5
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="3660" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-27580" yWindow="500" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1876,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="A1:E20"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1940,7 +1940,9 @@
       <c r="B4" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5">
+        <v>1.5972222222222224E-2</v>
+      </c>
       <c r="D4" s="2">
         <v>41805</v>
       </c>
@@ -1952,7 +1954,9 @@
       <c r="B5" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>3.125E-2</v>
+      </c>
       <c r="D5" s="2">
         <v>41805</v>
       </c>
@@ -1964,7 +1968,9 @@
       <c r="B6" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D6" s="2">
         <v>41805</v>
       </c>
@@ -1976,7 +1982,9 @@
       <c r="B7" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D7" s="2">
         <v>41805</v>
       </c>
@@ -1988,7 +1996,9 @@
       <c r="B8" s="1">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
       <c r="D8" s="2">
         <v>41805</v>
       </c>
@@ -2153,7 +2163,7 @@
       </c>
       <c r="C20" s="1">
         <f>SUM(C2:C19)</f>
-        <v>0.55625000000000002</v>
+        <v>0.6527777777777779</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -2172,7 +2182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made first reply, and reformatted code examples.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27580" yWindow="500" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-27580" yWindow="500" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -1876,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2182,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2246,7 +2246,9 @@
       <c r="B4" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5">
+        <v>2.4305555555555556E-2</v>
+      </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5">
@@ -2256,7 +2258,9 @@
       <c r="B5" s="1">
         <v>6.25E-2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>1.6666666666666666E-2</v>
+      </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5">
@@ -2266,7 +2270,9 @@
       <c r="B6" s="1">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5">
@@ -2336,7 +2342,9 @@
       <c r="B12" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D12" s="2">
         <v>41812</v>
       </c>
@@ -2411,7 +2419,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0.22777777777777775</v>
+        <v>0.31041666666666662</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Replied to another post.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27580" yWindow="500" windowWidth="24100" windowHeight="16380" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="34785" windowHeight="14970" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="week5" sheetId="5" r:id="rId5"/>
     <sheet name="week6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -155,11 +155,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -699,17 +699,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -973,17 +973,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1265,19 +1265,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1561,17 +1561,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1873,17 +1873,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2179,17 +2179,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2282,7 +2282,9 @@
       <c r="B7" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D7" s="2">
         <v>41812</v>
       </c>
@@ -2419,7 +2421,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0.31041666666666662</v>
+        <v>0.33124999999999993</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Took notes on week 6 lecture notes.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="34785" windowHeight="14970" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="11900" yWindow="2980" windowWidth="34780" windowHeight="14980" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="week5" sheetId="5" r:id="rId5"/>
     <sheet name="week6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -150,16 +150,19 @@
   </si>
   <si>
     <t>Read 19.9</t>
+  </si>
+  <si>
+    <t>Read up to page 13. It looks like pages 13-18 not needed for assignment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -699,17 +702,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -973,17 +976,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1265,19 +1268,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1561,17 +1564,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1873,17 +1876,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2179,17 +2182,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2247,7 +2250,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="C4" s="5">
-        <v>2.4305555555555556E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2262,6 +2265,9 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -2421,7 +2427,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0.33124999999999993</v>
+        <v>0.39930555555555547</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to 3rd post in DQ1
Still need to make at least one more in DQ2
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26640" yWindow="520" windowWidth="24660" windowHeight="17200" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="23445" windowHeight="11550" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="week5" sheetId="5" r:id="rId5"/>
     <sheet name="week6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -158,11 +158,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -702,17 +702,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -976,17 +976,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1268,19 +1268,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1564,17 +1564,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1876,17 +1876,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2182,17 +2182,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2316,7 +2316,9 @@
       <c r="B9" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D9" s="2">
         <v>41813</v>
       </c>
@@ -2431,7 +2433,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0.4409722222222221</v>
+        <v>0.46180555555555541</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made 3rd reply in week 6 DQ2
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2186,7 +2186,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2382,7 +2382,9 @@
       <c r="B14" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D14" s="2">
         <v>41813</v>
       </c>
@@ -2418,7 +2420,9 @@
       <c r="B17" s="1">
         <v>0.25</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D17" s="4">
         <v>41815</v>
       </c>
@@ -2433,7 +2437,7 @@
       </c>
       <c r="C18" s="1">
         <f>SUM(C2:C17)</f>
-        <v>0.46180555555555541</v>
+        <v>0.8159722222222221</v>
       </c>
       <c r="D18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Made week  7 schedule
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="23445" windowHeight="11550" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="18880" yWindow="3480" windowWidth="29700" windowHeight="19600" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="week4" sheetId="4" r:id="rId4"/>
     <sheet name="week5" sheetId="5" r:id="rId5"/>
     <sheet name="week6" sheetId="6" r:id="rId6"/>
+    <sheet name="week7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -153,16 +154,25 @@
   </si>
   <si>
     <t>Read up to page 13. It looks like pages 13-18 not needed for assignment.</t>
+  </si>
+  <si>
+    <t>Skim AJAX: Chapter 16</t>
+  </si>
+  <si>
+    <t>Skim HTML5: Chapter 14</t>
+  </si>
+  <si>
+    <t>Skim CSS3: Chapter 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,8 +222,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,7 +327,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -337,6 +365,15 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -374,6 +411,15 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -702,17 +748,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -976,17 +1022,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1268,19 +1314,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1564,17 +1610,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1876,17 +1922,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2182,17 +2228,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2440,6 +2486,265 @@
         <v>0.8159722222222221</v>
       </c>
       <c r="D18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2">
+        <v>41818</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41818</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4">
+        <v>41819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4">
+        <v>41822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <f>SUM(B2:B18)</f>
+        <v>0.85416666666666674</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Created skeleton of week 7 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="18880" yWindow="3480" windowWidth="29700" windowHeight="19600" tabRatio="500" activeTab="6"/>
@@ -2503,7 +2503,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2538,7 +2538,9 @@
       <c r="B2" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>4.6527777777777779E-2</v>
+      </c>
       <c r="D2" s="2">
         <v>41818</v>
       </c>

</xml_diff>

<commit_message>
Finished draft of week 7 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2539,7 +2539,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>4.6527777777777779E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D2" s="2">
         <v>41818</v>
@@ -2552,7 +2552,9 @@
       <c r="B3" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="D3" s="2">
         <v>41818</v>
       </c>

</xml_diff>

<commit_message>
Finished draft of week 7 DQ2
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2503,7 +2503,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2553,7 +2553,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>2.7777777777777776E-2</v>
+        <v>7.9166666666666663E-2</v>
       </c>
       <c r="D3" s="2">
         <v>41818</v>

</xml_diff>

<commit_message>
Responded to first post for week 7
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18880" yWindow="3480" windowWidth="29700" windowHeight="19600" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-28740" yWindow="60" windowWidth="29700" windowHeight="19600" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -2503,7 +2503,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2614,7 +2614,9 @@
       <c r="B8" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D8" s="2">
         <v>41819</v>
       </c>

</xml_diff>

<commit_message>
responded to 2 more posts.
responded to 2 more posts.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28740" yWindow="60" windowWidth="29700" windowHeight="19600" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="32460" windowHeight="12495" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="week6" sheetId="6" r:id="rId6"/>
     <sheet name="week7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -168,11 +168,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -748,17 +748,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1022,17 +1022,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1314,19 +1314,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1610,17 +1610,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1922,17 +1922,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2228,17 +2228,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2499,17 +2499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2628,7 +2628,9 @@
       <c r="B9" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D9" s="2">
         <v>41820</v>
       </c>
@@ -2676,7 +2678,9 @@
       <c r="B13" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="D13" s="4">
         <v>41819</v>
       </c>
@@ -2736,7 +2740,9 @@
       <c r="B18" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>0.25</v>
+      </c>
       <c r="D18" s="4">
         <v>41822</v>
       </c>
@@ -2749,7 +2755,10 @@
         <f>SUM(B2:B18)</f>
         <v>0.85416666666666674</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <f>SUM(C2:C18)</f>
+        <v>0.48194444444444451</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 posts to each DQ
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2503,7 +2503,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2642,7 +2642,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41821</v>
       </c>
@@ -2692,7 +2694,9 @@
       <c r="B14" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D14" s="2">
         <v>41820</v>
       </c>
@@ -2704,7 +2708,9 @@
       <c r="B15" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="D15" s="2">
         <v>41821</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C18" s="1">
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D18" s="4">
         <v>41822</v>
@@ -2757,7 +2763,7 @@
       </c>
       <c r="C19" s="1">
         <f>SUM(C2:C18)</f>
-        <v>0.48194444444444451</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="D19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Started week 8 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="32460" windowHeight="12495" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="15160" yWindow="3160" windowWidth="32620" windowHeight="20900" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,9 @@
     <sheet name="week5" sheetId="5" r:id="rId5"/>
     <sheet name="week6" sheetId="6" r:id="rId6"/>
     <sheet name="week7" sheetId="7" r:id="rId7"/>
+    <sheet name="week8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -168,11 +169,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,8 +223,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -327,7 +340,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -374,6 +387,12 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -420,6 +439,12 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,17 +773,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1022,17 +1047,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1314,19 +1339,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1610,17 +1635,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1922,17 +1947,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2228,17 +2253,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2499,17 +2524,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2766,6 +2791,236 @@
         <v>0.72500000000000009</v>
       </c>
       <c r="D19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>41824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>41825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>41825</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>41826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>41827</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <f>D7+1</f>
+        <v>41828</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <f>D8+1</f>
+        <v>41829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2">
+        <v>41825</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2">
+        <v>41826</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>41827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2">
+        <f>D12+1</f>
+        <v>41828</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2">
+        <f>D13+1</f>
+        <v>41829</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4">
+        <v>41829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
+        <v>0.76041666666666685</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUM(C2:C15)</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Did critique of our website.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2844,7 +2844,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="2">
         <v>41824</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished skeleton of week 8 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2807,7 +2807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2844,7 +2844,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="D2" s="2">
         <v>41824</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Submitted week 8 DQ1
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2844,7 +2844,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C2" s="1">
-        <v>9.7222222222222224E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="D2" s="2">
         <v>41824</v>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>9.7222222222222224E-2</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished draft of week 8 DQ2
Still need to proofread.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2858,7 +2858,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="C3" s="1">
-        <v>3.472222222222222E-3</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="D3" s="2">
         <v>41825</v>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>0.13680555555555554</v>
+        <v>0.20624999999999999</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Responded to first post.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15160" yWindow="3160" windowWidth="32620" windowHeight="20900" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="1770" yWindow="2625" windowWidth="21120" windowHeight="9645" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="week1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="week7" sheetId="7" r:id="rId7"/>
     <sheet name="week8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -169,11 +169,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -773,17 +773,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C19" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1047,17 +1047,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A16" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1339,19 +1339,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1635,17 +1635,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1947,17 +1947,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2253,17 +2253,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2524,17 +2524,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2804,17 +2804,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2943,7 +2943,9 @@
       <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D10" s="2">
         <v>41825</v>
       </c>
@@ -3020,7 +3022,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>0.20624999999999999</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>

<commit_message>
Now have 4 replies to each DQ
Make one more for each if time allows.
</commit_message>
<xml_diff>
--- a/InternetProg__tasksCompletion.xlsx
+++ b/InternetProg__tasksCompletion.xlsx
@@ -2807,7 +2807,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2992,7 +2992,9 @@
       <c r="B13" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D13" s="2">
         <f>D12+1</f>
         <v>41828</v>
@@ -3018,7 +3020,9 @@
       <c r="B15" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="D15" s="4">
         <v>41829</v>
       </c>
@@ -3033,7 +3037,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUM(C2:C15)</f>
-        <v>0.30694444444444446</v>
+        <v>0.53611111111111109</v>
       </c>
       <c r="D16" s="2"/>
     </row>

</xml_diff>